<commit_message>
25-09-19 2a Visualización corregida y completa.
</commit_message>
<xml_diff>
--- a/data/afiliaciones/09_CDMX.xlsx
+++ b/data/afiliaciones/09_CDMX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Salamandra/afiliacion/data/afiliaciones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2969C88-6016-7C49-9DDF-0B93A31D6344}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E1B3CC-F0A4-5544-A29E-954B9EC9B612}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1178,7 +1178,7 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1327,7 +1327,7 @@
         <v>1245</v>
       </c>
       <c r="O3" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="P3" t="s">
         <v>26</v>
@@ -1627,7 +1627,7 @@
         <v>3214</v>
       </c>
       <c r="O9" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="P9" t="s">
         <v>52</v>
@@ -1777,7 +1777,7 @@
         <v>1023</v>
       </c>
       <c r="O12" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="P12" t="s">
         <v>64</v>
@@ -1877,7 +1877,7 @@
         <v>1478</v>
       </c>
       <c r="O14" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="P14" t="s">
         <v>72</v>
@@ -1927,7 +1927,7 @@
         <v>3014</v>
       </c>
       <c r="O15" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="P15" t="s">
         <v>76</v>
@@ -2027,7 +2027,7 @@
         <v>2587</v>
       </c>
       <c r="O17" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="P17" t="s">
         <v>84</v>

</xml_diff>